<commit_message>
Add tournament from Vadim and Vladimir
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python\SI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5589B46D-F110-40C4-AF58-1429223DDFA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D99757C5-3BCC-4A8F-A29C-F39D7BC26661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Players" sheetId="15" r:id="rId1"/>
@@ -21,13 +21,14 @@
     <sheet name="Vuelta_2" sheetId="13" r:id="rId6"/>
     <sheet name="Nevermore_1" sheetId="21" r:id="rId7"/>
     <sheet name="Nevermore_2" sheetId="19" r:id="rId8"/>
+    <sheet name="BG_1" sheetId="22" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1044" uniqueCount="68">
   <si>
     <t>Вадим Барановский</t>
   </si>
@@ -355,7 +356,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -388,6 +389,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -636,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3ECE8D9-B069-4F85-B251-FD53E1070CE4}">
   <dimension ref="A1:B68"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -8419,7 +8428,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C6422A9-EE8D-4F84-A5AA-CE6E72B89389}">
   <dimension ref="A1:B56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
@@ -8820,4 +8829,557 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1106E9D-E33E-420C-AEDD-C2A0BC8F036A}">
+  <dimension ref="A1:D70"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="I41" sqref="I41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2"/>
+  <cols>
+    <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15">
+      <c r="A1" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="20">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15">
+      <c r="A2" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="20">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15">
+      <c r="A3" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="20">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15">
+      <c r="A4" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="20">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="18" customFormat="1" ht="15">
+      <c r="A5" s="19"/>
+      <c r="B5" s="20"/>
+    </row>
+    <row r="6" spans="1:4" s="18" customFormat="1" ht="15">
+      <c r="A6" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="20">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="18" customFormat="1" ht="15">
+      <c r="A7" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="20">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="18" customFormat="1" ht="15">
+      <c r="A8" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="20">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="18" customFormat="1" ht="15">
+      <c r="A9" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="20">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="18" customFormat="1" ht="15">
+      <c r="A10" s="19"/>
+      <c r="B10" s="20"/>
+    </row>
+    <row r="11" spans="1:4" ht="15">
+      <c r="A11" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="20">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15">
+      <c r="A12" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="20">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15">
+      <c r="A13" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="20">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15">
+      <c r="A14" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="20">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="18" customFormat="1" ht="15">
+      <c r="A15" s="19"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="20"/>
+    </row>
+    <row r="16" spans="1:4" s="18" customFormat="1" ht="15">
+      <c r="A16" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="20">
+        <v>10</v>
+      </c>
+      <c r="C16" s="19"/>
+      <c r="D16" s="20"/>
+    </row>
+    <row r="17" spans="1:4" s="18" customFormat="1" ht="15">
+      <c r="A17" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="20">
+        <v>140</v>
+      </c>
+      <c r="C17" s="19"/>
+      <c r="D17" s="20"/>
+    </row>
+    <row r="18" spans="1:4" s="18" customFormat="1" ht="15">
+      <c r="A18" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="20">
+        <v>10</v>
+      </c>
+      <c r="C18" s="19"/>
+      <c r="D18" s="20"/>
+    </row>
+    <row r="19" spans="1:4" s="18" customFormat="1" ht="15">
+      <c r="A19" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="20">
+        <v>50</v>
+      </c>
+      <c r="C19" s="19"/>
+      <c r="D19" s="20"/>
+    </row>
+    <row r="20" spans="1:4" s="18" customFormat="1" ht="15">
+      <c r="A20" s="19"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="20"/>
+    </row>
+    <row r="21" spans="1:4" s="18" customFormat="1" ht="15">
+      <c r="A21" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="20">
+        <v>-10</v>
+      </c>
+      <c r="C21" s="19"/>
+      <c r="D21" s="20"/>
+    </row>
+    <row r="22" spans="1:4" s="18" customFormat="1" ht="15">
+      <c r="A22" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="20">
+        <v>90</v>
+      </c>
+      <c r="C22" s="19"/>
+      <c r="D22" s="20"/>
+    </row>
+    <row r="23" spans="1:4" s="18" customFormat="1" ht="15">
+      <c r="A23" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="20">
+        <v>30</v>
+      </c>
+      <c r="C23" s="19"/>
+      <c r="D23" s="20"/>
+    </row>
+    <row r="24" spans="1:4" ht="15">
+      <c r="A24" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" s="20">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="18" customFormat="1" ht="15">
+      <c r="A25" s="19"/>
+      <c r="B25" s="20"/>
+    </row>
+    <row r="26" spans="1:4" s="18" customFormat="1" ht="15">
+      <c r="A26" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="20">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="18" customFormat="1" ht="15">
+      <c r="A27" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="20">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" s="18" customFormat="1" ht="15">
+      <c r="A28" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" s="20">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" s="18" customFormat="1" ht="15">
+      <c r="A29" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="20">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" s="18" customFormat="1" ht="15">
+      <c r="A30" s="19"/>
+      <c r="B30" s="20"/>
+    </row>
+    <row r="31" spans="1:4" s="18" customFormat="1" ht="15">
+      <c r="A31" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" s="20">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" s="18" customFormat="1" ht="15">
+      <c r="A32" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="20">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" s="18" customFormat="1" ht="15">
+      <c r="A33" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" s="20">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" s="18" customFormat="1" ht="15">
+      <c r="A34" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" s="20">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" s="18" customFormat="1" ht="15">
+      <c r="A35" s="19"/>
+      <c r="B35" s="20"/>
+    </row>
+    <row r="36" spans="1:2" ht="15">
+      <c r="A36" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36" s="20">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="15">
+      <c r="A37" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B37" s="20">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" s="18" customFormat="1" ht="15">
+      <c r="A38" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B38" s="20">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" s="18" customFormat="1" ht="15">
+      <c r="A39" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B39" s="20">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" s="18" customFormat="1">
+      <c r="A40" s="21"/>
+      <c r="B40" s="21"/>
+    </row>
+    <row r="41" spans="1:2" s="18" customFormat="1" ht="15">
+      <c r="A41" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41" s="20">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" s="18" customFormat="1" ht="15">
+      <c r="A42" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B42" s="20">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" s="18" customFormat="1" ht="15">
+      <c r="A43" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B43" s="20">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" s="18" customFormat="1" ht="15">
+      <c r="A44" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44" s="20">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" s="18" customFormat="1">
+      <c r="A45" s="21"/>
+      <c r="B45" s="21"/>
+    </row>
+    <row r="46" spans="1:2" s="18" customFormat="1" ht="15">
+      <c r="A46" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B46" s="20">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" s="18" customFormat="1" ht="15">
+      <c r="A47" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B47" s="20">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" s="18" customFormat="1" ht="15">
+      <c r="A48" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B48" s="20">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" s="18" customFormat="1" ht="15">
+      <c r="A49" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B49" s="20">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" s="18" customFormat="1" ht="15">
+      <c r="A50" s="19"/>
+      <c r="B50" s="20"/>
+    </row>
+    <row r="51" spans="1:4" ht="15">
+      <c r="A51" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B51" s="20">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="13.2" customHeight="1">
+      <c r="A52" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B52" s="20">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="15">
+      <c r="A53" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B53" s="20">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="15">
+      <c r="A54" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B54" s="20">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" s="18" customFormat="1" ht="15">
+      <c r="A55" s="19"/>
+      <c r="B55" s="20"/>
+      <c r="C55" s="19"/>
+      <c r="D55" s="20"/>
+    </row>
+    <row r="56" spans="1:4" s="18" customFormat="1" ht="15">
+      <c r="A56" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B56" s="20">
+        <v>60</v>
+      </c>
+      <c r="C56" s="19"/>
+      <c r="D56" s="20"/>
+    </row>
+    <row r="57" spans="1:4" s="18" customFormat="1" ht="15">
+      <c r="A57" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B57" s="20">
+        <v>180</v>
+      </c>
+      <c r="C57" s="19"/>
+      <c r="D57" s="20"/>
+    </row>
+    <row r="58" spans="1:4" s="18" customFormat="1" ht="15">
+      <c r="A58" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B58" s="20">
+        <v>250</v>
+      </c>
+      <c r="C58" s="19"/>
+      <c r="D58" s="20"/>
+    </row>
+    <row r="59" spans="1:4" s="18" customFormat="1" ht="15">
+      <c r="A59" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B59" s="20">
+        <v>30</v>
+      </c>
+      <c r="C59" s="19"/>
+      <c r="D59" s="20"/>
+    </row>
+    <row r="60" spans="1:4" s="18" customFormat="1" ht="15">
+      <c r="A60" s="19"/>
+      <c r="B60" s="20"/>
+      <c r="C60" s="19"/>
+      <c r="D60" s="20"/>
+    </row>
+    <row r="61" spans="1:4" ht="15">
+      <c r="A61" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B61" s="20">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="15">
+      <c r="A62" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B62" s="20">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="15">
+      <c r="A63" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B63" s="20">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="15">
+      <c r="A64" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B64" s="20">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="21"/>
+      <c r="B65" s="21"/>
+    </row>
+    <row r="66" spans="1:2" ht="15">
+      <c r="A66" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B66" s="20">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="15">
+      <c r="A67" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B67" s="20">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="15">
+      <c r="A68" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B68" s="20">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="15">
+      <c r="A69" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B69" s="20">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" s="18" customFormat="1" ht="15">
+      <c r="A70" s="19"/>
+      <c r="B70" s="20"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>